<commit_message>
With video example trials
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/mel_production/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EFF818-7B5D-0840-9AB6-1912BF4E9238}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7966ABBC-B88A-9A41-8620-AF4B602092DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="460" windowWidth="36860" windowHeight="19200" xr2:uid="{F918617E-B214-614F-96D8-792A3F23E788}"/>
+    <workbookView xWindow="4440" yWindow="1040" windowWidth="35840" windowHeight="19200" xr2:uid="{F918617E-B214-614F-96D8-792A3F23E788}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="94">
   <si>
     <t>id</t>
   </si>
@@ -47,9 +47,6 @@
     <t>text</t>
   </si>
   <si>
-    <t>&lt;p&gt; Welcome to the &lt;strong&gt;Melody Singing Test!&lt;/strong&gt; &lt;/p&gt; &lt;br&gt; &lt;p&gt; Please click below to proceed. &lt;/p&gt;</t>
-  </si>
-  <si>
     <t>button_text</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>Give Browser Info</t>
   </si>
   <si>
-    <t>&lt;p&gt;Now we need to record you humming any comfortable note for 5 seconds.&lt;/p&gt; &lt;p&gt;Feel free to practice first: try to keep one long hum without stopping.&lt;/p&gt; &lt;p&gt;When you are ready, take a deep breath, start humming, and then click the Ready button just after.&lt;/p&gt; &lt;p&gt; You can stop humming when the red bird disappears.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Please sing "Happy Birthday" using the following lyrics and name:&lt;/p&gt; &lt;p&gt; Happy birthday to you. Happy birthday to you. Happy birthday to Alex. Happy birthday to you. &lt;/p&gt; &lt;p&gt;Press Stop when you are finished&lt;/p&gt;</t>
   </si>
   <si>
@@ -182,9 +176,6 @@
     <t>&lt;p&gt;We care about your privacy, so on this page we need you to let us do two things:&lt;/p&gt;&lt;ol&gt;&lt;li&gt; Please click Allow on the popup message to let us record you for this experiment. &lt;/li&gt;&lt;li&gt;Click Give Browser Info to give us information about your browser.&lt;li&gt;&lt;p&gt; We need this to ensure that your setup is okay for this experiment.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;We need to test your microphone before we proceed.&lt;/p&gt;&lt;p&gt; Please make sure your microphone is plugged in then click below. &lt;/p&gt;&lt;p&gt;You should see the levels change below as you make sound. If you do not, then your microphone may not be setup properly and you will need to try again.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>other</t>
   </si>
   <si>
@@ -212,9 +203,6 @@
     <t>Berkowitz</t>
   </si>
   <si>
-    <t>max</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Press Play to hear a melody.&lt;/p&gt;&lt;p&gt; Try and sing back the melody plus the rhythm as best you can. Just do your best on the first try then press stop. Do not worry if you think you got it wrong.</t>
   </si>
   <si>
@@ -230,9 +218,6 @@
     <t>Yes, I am wearing headphones./I cannot use headphones.</t>
   </si>
   <si>
-    <t>&lt;p&gt;We need to record 5 seconds of your room &lt;strong&gt;without&lt;/strong&gt; with you being quiet to see what your background noise is like.&lt;/p&gt;&lt;p&gt; When you are ready to record your environment for 5 seconds, press the button below.&lt;/p&gt; &lt;p&gt;Please try &lt;strong&gt; not &lt;/strong&gt; to make a noise! &lt;/p&gt;</t>
-  </si>
-  <si>
     <t>I'm Ready To Record My Background</t>
   </si>
   <si>
@@ -243,13 +228,100 @@
   </si>
   <si>
     <t>Play Two Notes</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Welcome to the &lt;strong&gt;Melody Singing Test!&lt;/strong&gt; &lt;/p&gt; &lt;p&gt; Please click below to proceed. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We need to record 5 seconds of your room &lt;strong&gt;with you being quiet&lt;/strong&gt; to see what your background noise is like.&lt;/p&gt;&lt;p&gt; When you are ready to record your environment for 5 seconds, press the button below.&lt;/p&gt; &lt;p&gt;Please try &lt;strong&gt; not &lt;/strong&gt; to make a noise! &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>example_1</t>
+  </si>
+  <si>
+    <t>example_2</t>
+  </si>
+  <si>
+    <t>example_8</t>
+  </si>
+  <si>
+    <t>example_7</t>
+  </si>
+  <si>
+    <t>example_6</t>
+  </si>
+  <si>
+    <t>example_5</t>
+  </si>
+  <si>
+    <t>example_4</t>
+  </si>
+  <si>
+    <t>example_3</t>
+  </si>
+  <si>
+    <t>video_page</t>
+  </si>
+  <si>
+    <t>src = "video/Example_2.mp4"</t>
+  </si>
+  <si>
+    <t>src = "video/Example_1.mp4"</t>
+  </si>
+  <si>
+    <t>src = "video/Example_3.mp4"</t>
+  </si>
+  <si>
+    <t>src = "video/Example_4.mp4"</t>
+  </si>
+  <si>
+    <t>src = "video/Example_5.mp4"</t>
+  </si>
+  <si>
+    <t>src = "video/Example_6.mp4"</t>
+  </si>
+  <si>
+    <t>src = "video/Example_7.mp4"</t>
+  </si>
+  <si>
+    <t>src = "video/Example_8.mp4"</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; On the next screen, you will need to record 5 seconds of your room whilst being quiet.&lt;/p&gt;&lt;p&gt; Click to watch how to complete the next screen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; On the next screen, you will need to test if your microphone works&lt;/p&gt;&lt;p&gt; Click to watch how to complete the next screen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; On the next screen, you will need to hum or say "aah"&lt;/p&gt;&lt;p&gt; Click to watch how to complete the next screen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Now we need to record you humming or "aaahing" any comfortable note for 5 seconds.&lt;/p&gt; &lt;p&gt;Feel free to practice first: try to keep one long hum without stopping.&lt;/p&gt; &lt;p&gt;When you are ready, take a deep breath, start humming, and then click the Ready button just after.&lt;/p&gt; &lt;p&gt; You can stop humming when the red bird disappears.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; On the next screen, you will need to sing Happy Birthday from a comfortable note.&lt;/p&gt;&lt;p&gt; Click to watch how to complete the next screen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; On the next screen, you will need to sing along with a note.&lt;/p&gt;&lt;p&gt; Click to watch how to complete the next screen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; On the next screen, you will need to sing back two notes you hear.&lt;/p&gt;&lt;p&gt; Click to watch how to complete the next screen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;On the next screen, you will need to sing back a melody you hear.&lt;/p&gt;&lt;p&gt; Click to watch how to complete the next screen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; On the next screen, you will need to sing back a melody, but this time you can take as long as you need.&lt;/p&gt;&lt;p&gt; Click to watch how to complete the next screen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We need to test your microphone before we proceed.&lt;/p&gt;&lt;p&gt; Please make sure your microphone is plugged in then click below. &lt;/p&gt;&lt;p&gt;You should see the levels change below as you make sound. If you do not, then your microphone may not be setup properly.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -270,6 +342,13 @@
       <color rgb="FF222222"/>
       <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -292,12 +371,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF35A9C-231E-5348-9328-9A574E33D2C7}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -638,25 +721,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -664,27 +747,27 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2" s="3" t="b">
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -693,21 +776,21 @@
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -716,98 +799,104 @@
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F6" s="3" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>75</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="F7" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>49</v>
+      <c r="H7" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>75</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="F9" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -815,148 +904,302 @@
         <v>40</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F10" s="3" t="b">
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>39</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1</v>
-      </c>
-      <c r="F11" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>13</v>
+        <v>75</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="3">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F12" s="3" t="b">
         <v>1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="3">
-        <v>2</v>
-      </c>
-      <c r="F13" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="3">
-        <v>2</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="3">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="F14" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="H14" s="2" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>34</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>53</v>
+        <v>75</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>33</v>
+        <v>26</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
       </c>
       <c r="F16" s="3" t="b">
         <v>1</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="3" t="s">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>55</v>
+      </c>
+      <c r="E20" s="3">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3">
+        <v>4</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="3">
+        <v>2</v>
+      </c>
+      <c r="F22" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3">
+        <v>8</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working saved user range feature (but needs comprehensive testing)
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/mel_production/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7966ABBC-B88A-9A41-8620-AF4B602092DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B664A167-A0D9-0D47-85BA-1BA98F152DDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1040" windowWidth="35840" windowHeight="19200" xr2:uid="{F918617E-B214-614F-96D8-792A3F23E788}"/>
+    <workbookView xWindow="0" yWindow="1280" windowWidth="35840" windowHeight="19200" xr2:uid="{F918617E-B214-614F-96D8-792A3F23E788}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
   <si>
     <t>id</t>
   </si>
@@ -50,9 +50,6 @@
     <t>button_text</t>
   </si>
   <si>
-    <t>I'm Ready</t>
-  </si>
-  <si>
     <t>NAFC_page</t>
   </si>
   <si>
@@ -167,24 +164,15 @@
     <t>&lt;p&gt;Are you in a quiet environment?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;To complete this test you must wear headphones. &lt;/p&gt;Please do not playback sound through your speakers.&lt;/p&gt;&lt;p&gt; Please confirm that you will use headphones.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;You should hear some audio playing.&lt;/p&gt;&lt;p&gt; Please adjust the volume to a comfortable level before continuing.&lt;/p&gt; &lt;p&gt;If you cannot make the audio play at a comfortable level, please do not continue, but instead contact the researcher for help.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;We care about your privacy, so on this page we need you to let us do two things:&lt;/p&gt;&lt;ol&gt;&lt;li&gt; Please click Allow on the popup message to let us record you for this experiment. &lt;/li&gt;&lt;li&gt;Click Give Browser Info to give us information about your browser.&lt;li&gt;&lt;p&gt; We need this to ensure that your setup is okay for this experiment.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>other</t>
   </si>
   <si>
     <t>url = "audio/test_headphones.mp3"</t>
   </si>
   <si>
-    <t>&lt;p&gt;Please describe any other issues you experienced runwith the test.</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Were all the instructions easy to understand? If not, please described what confused you.&lt;/p&gt;</t>
   </si>
   <si>
@@ -230,9 +218,6 @@
     <t>Play Two Notes</t>
   </si>
   <si>
-    <t>&lt;p&gt; Welcome to the &lt;strong&gt;Melody Singing Test!&lt;/strong&gt; &lt;/p&gt; &lt;p&gt; Please click below to proceed. &lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;We need to record 5 seconds of your room &lt;strong&gt;with you being quiet&lt;/strong&gt; to see what your background noise is like.&lt;/p&gt;&lt;p&gt; When you are ready to record your environment for 5 seconds, press the button below.&lt;/p&gt; &lt;p&gt;Please try &lt;strong&gt; not &lt;/strong&gt; to make a noise! &lt;/p&gt;</t>
   </si>
   <si>
@@ -290,21 +275,12 @@
     <t>&lt;p&gt; On the next screen, you will need to record 5 seconds of your room whilst being quiet.&lt;/p&gt;&lt;p&gt; Click to watch how to complete the next screen.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt; On the next screen, you will need to test if your microphone works&lt;/p&gt;&lt;p&gt; Click to watch how to complete the next screen.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt; On the next screen, you will need to hum or say "aah"&lt;/p&gt;&lt;p&gt; Click to watch how to complete the next screen.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Now we need to record you humming or "aaahing" any comfortable note for 5 seconds.&lt;/p&gt; &lt;p&gt;Feel free to practice first: try to keep one long hum without stopping.&lt;/p&gt; &lt;p&gt;When you are ready, take a deep breath, start humming, and then click the Ready button just after.&lt;/p&gt; &lt;p&gt; You can stop humming when the red bird disappears.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt; On the next screen, you will need to sing Happy Birthday from a comfortable note.&lt;/p&gt;&lt;p&gt; Click to watch how to complete the next screen.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt; On the next screen, you will need to sing along with a note.&lt;/p&gt;&lt;p&gt; Click to watch how to complete the next screen.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt; On the next screen, you will need to sing back two notes you hear.&lt;/p&gt;&lt;p&gt; Click to watch how to complete the next screen.&lt;/p&gt;</t>
   </si>
   <si>
@@ -314,7 +290,67 @@
     <t>&lt;p&gt; On the next screen, you will need to sing back a melody, but this time you can take as long as you need.&lt;/p&gt;&lt;p&gt; Click to watch how to complete the next screen.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;We need to test your microphone before we proceed.&lt;/p&gt;&lt;p&gt; Please make sure your microphone is plugged in then click below. &lt;/p&gt;&lt;p&gt;You should see the levels change below as you make sound. If you do not, then your microphone may not be setup properly.&lt;/p&gt;</t>
+    <t>&lt;p&gt; On the next screen, you will need to hum or say "aah".&lt;/p&gt;&lt;p&gt; Click to watch how to complete the next screen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;On the next screen, you will need to test if your microphone works&lt;/p&gt;&lt;p&gt; Click to watch how to complete the next screen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; For the first round of trials, you will need to sing &lt;strong&gt;along&lt;/strong&gt; with a note that you hear.&lt;/p&gt;&lt;p&gt; Click to watch how to complete the next screen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>start_test</t>
+  </si>
+  <si>
+    <t>instructions</t>
+  </si>
+  <si>
+    <t>instructions_2</t>
+  </si>
+  <si>
+    <t>instructions_3</t>
+  </si>
+  <si>
+    <t>mic_question</t>
+  </si>
+  <si>
+    <t>In-Built/Plugged-In</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Please describe any other issues you experienced.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Welcome to the &lt;strong&gt;Melody Singing Task!&lt;/strong&gt; &lt;/p&gt; &lt;p&gt; Please click below to proceed. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;To complete this task you must wear headphones. &lt;/p&gt;Please do not playback sound through your speakers.&lt;/p&gt;&lt;p&gt; Please confirm that you will use headphones.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; The idea of this task is to get you singing back melodies we play to you. &lt;p&gt;We will play the melodies in different ways, so it is important that you understand what you are doing before you proceed with each round. &lt;/p&gt;&lt;p&gt;Please read the instructions carefully!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;It is fine if you do not think you are a good singer. &lt;/p&gt;&lt;p&gt;In fact, one reason why we study musical abilities is so that we can help people the struggle improve them. &lt;/p&gt;&lt;p&gt;Just do your best and have fun!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; You will need the following: &lt;/p&gt; &lt;ol&gt;&lt;li&gt;A quiet space&lt;/li&gt;&lt;li&gt;A pair of headphones&lt;/li&gt;&lt;li&gt;A microphone*&lt;/li&gt;&lt;/ol&gt; &lt;p style="font-size:12px";&gt; NB: A microphone in-built into your computer is acceptable, but please use a plugged in microphone which is quite close to your mouth if you can&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Are you using a plugged-in or in-built microphone?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We care about your privacy, so on this page we need you to let us do two things:&lt;/p&gt;&lt;ol&gt;&lt;li&gt; Please click Allow on the popup message to let us record you for this experiment. &lt;/li&gt;&lt;li&gt;Click Give Browser Info to give us information about your browser.&lt;li&gt;&lt;/ol&gt;&lt;p&gt; We need this to ensure that your setup is okay for this experiment.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We need to test your microphone before we proceed.&lt;/p&gt;&lt;p&gt; Please make sure your microphone is plugged in then click on the microphone image. &lt;/p&gt;&lt;p&gt;You should see the levels change below as you make sound. If you do not, then your microphone may not be setup properly.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Okay, now everything is setup! Click to proceed to the main tasks.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>instructions_4</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Well done! You have completed all the main singing tasks, but please answer a few questions on the next couple of pages.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -695,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF35A9C-231E-5348-9328-9A574E33D2C7}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="103" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -721,19 +757,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
@@ -747,433 +783,413 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="3" t="b">
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+        <v>89</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="F3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G3" s="4"/>
       <c r="H3" s="2" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="F4" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G4" s="4"/>
       <c r="H4" s="2" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="F5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="3" t="b">
+      <c r="I6" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="G8" s="5"/>
       <c r="H8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="F9" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>84</v>
+      <c r="H9" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F10" s="3" t="b">
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>74</v>
+      <c r="A11" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" s="5" t="b">
+        <v>70</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="3" t="b">
         <v>0</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>86</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F12" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>73</v>
+      <c r="A13" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>88</v>
-      </c>
       <c r="I13" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F14" s="3" t="b">
         <v>1</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F15" s="5" t="b">
         <v>0</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F16" s="3" t="b">
         <v>1</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>90</v>
-      </c>
       <c r="I17" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="3">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="F18" s="3" t="b">
         <v>1</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C20" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="F20" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" s="3">
-        <v>2</v>
-      </c>
-      <c r="F20" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G20" s="3">
-        <v>4</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F21" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="3">
-        <v>2</v>
-      </c>
-      <c r="F22" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G22" s="3">
-        <v>8</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="I22" s="3" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
       </c>
       <c r="F23" s="3" t="b">
         <v>1</v>
@@ -1182,24 +1198,154 @@
         <v>50</v>
       </c>
       <c r="I23" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="3">
+        <v>2</v>
+      </c>
+      <c r="F25" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3">
+        <v>4</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="I25" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="3">
+        <v>2</v>
+      </c>
+      <c r="F27" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3">
+        <v>8</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="3" t="b">
+      <c r="B29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>52</v>
+      <c r="H29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>